<commit_message>
Versão final Projeto individual
</commit_message>
<xml_diff>
--- a/Documentação/sprint backlog.xlsx
+++ b/Documentação/sprint backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/lucas_teixeira_bandtec_com_br/Documents/Desktop/Github/projeto-individual-imagine-dragons/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65EC7BF4-99F5-442E-BFCB-82253E1D2F72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{65EC7BF4-99F5-442E-BFCB-82253E1D2F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3749035B-000B-450A-874F-2E0D216C9E41}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{03BB0B3A-0AB5-49F3-81D6-DC877D290CD2}"/>
+    <workbookView xWindow="16284" yWindow="-1764" windowWidth="19416" windowHeight="10416" xr2:uid="{03BB0B3A-0AB5-49F3-81D6-DC877D290CD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,7 +241,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.249977111117893"/>
+        <fgColor theme="2" tint="-0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -627,49 +627,130 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -681,13 +762,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -699,87 +777,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1106,50 +1104,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2569F6F-DBCD-41B7-BB20-F68246BD3BDD}">
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="35"/>
-    <col min="6" max="6" width="18.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="35"/>
+    <col min="1" max="1" width="2.85546875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="40"/>
+    <col min="6" max="6" width="18.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="46"/>
+      <c r="C2" s="47"/>
     </row>
     <row r="3" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="32" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1163,16 +1161,16 @@
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="18">
         <v>13</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="14">
         <v>44325</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="48">
         <f>SUM(E4:E11)</f>
         <v>45</v>
       </c>
@@ -1181,541 +1179,541 @@
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8">
         <v>3</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>2</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="15">
         <v>44326</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="D6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="19">
         <v>13</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="11">
         <v>3</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <v>44327</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="D7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="8">
         <v>1</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>4</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="15">
         <v>44327</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="49"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="D8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="19">
         <v>1</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="11">
         <v>5</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <v>44328</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="49"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="8">
         <v>2</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>6</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="15">
         <v>44329</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="D10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="8">
         <v>5</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>7</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="15">
         <v>44330</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="15">
+      <c r="D11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="20">
         <v>7</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="13">
         <v>8</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="17">
         <v>44330</v>
       </c>
-      <c r="H11" s="23"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="13" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="51"/>
+      <c r="C13" s="52"/>
     </row>
     <row r="14" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="49" t="s">
+      <c r="H14" s="35" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="30">
+      <c r="D15" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="24">
         <v>8</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="24">
         <v>1</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="25">
         <v>44333</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="53">
         <f>SUM(E15:E21)</f>
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="30">
+      <c r="D16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="24">
         <v>13</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="24">
         <v>2</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="25">
         <v>44333</v>
       </c>
-      <c r="H16" s="28"/>
+      <c r="H16" s="54"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="24">
         <v>2</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="24">
         <v>3</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="25">
         <v>44334</v>
       </c>
-      <c r="H17" s="28"/>
+      <c r="H17" s="54"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="30">
+      <c r="D18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="24">
         <v>21</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="24">
         <v>4</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="25">
         <v>44336</v>
       </c>
-      <c r="H18" s="28"/>
+      <c r="H18" s="54"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="30">
+      <c r="D19" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="24">
         <v>5</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="24">
         <v>5</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="25">
         <v>44336</v>
       </c>
-      <c r="H19" s="28"/>
+      <c r="H19" s="54"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="30">
+      <c r="D20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="24">
         <v>13</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="24">
         <v>6</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="25">
         <v>44338</v>
       </c>
-      <c r="H20" s="29"/>
+      <c r="H20" s="55"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="39"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
       <c r="H21" s="38"/>
     </row>
     <row r="22" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
       <c r="H22" s="38"/>
     </row>
     <row r="23" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="41" t="s">
+      <c r="G23" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="52" t="s">
+      <c r="H23" s="36" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="40">
+      <c r="D24" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="28">
         <v>5</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="28">
         <v>1</v>
       </c>
-      <c r="G24" s="57">
+      <c r="G24" s="37">
         <v>44342</v>
       </c>
-      <c r="H24" s="53">
+      <c r="H24" s="41">
         <f>SUM(E24:E32)</f>
         <v>97</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="40">
+      <c r="D25" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="28">
         <v>5</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="28">
         <v>2</v>
       </c>
-      <c r="G25" s="57">
+      <c r="G25" s="37">
         <v>44343</v>
       </c>
-      <c r="H25" s="58"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="28">
         <v>21</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="28">
         <v>2</v>
       </c>
-      <c r="G26" s="57">
+      <c r="G26" s="37">
         <v>44344</v>
       </c>
-      <c r="H26" s="54"/>
+      <c r="H26" s="43"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="40">
+      <c r="E27" s="28">
         <v>13</v>
       </c>
-      <c r="F27" s="40">
+      <c r="F27" s="28">
         <v>3</v>
       </c>
-      <c r="G27" s="57">
+      <c r="G27" s="37">
         <v>44344</v>
       </c>
-      <c r="H27" s="54"/>
+      <c r="H27" s="43"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="40">
+      <c r="D28" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="28">
         <v>8</v>
       </c>
-      <c r="F28" s="40">
+      <c r="F28" s="28">
         <v>4</v>
       </c>
-      <c r="G28" s="57">
+      <c r="G28" s="37">
         <v>44344</v>
       </c>
-      <c r="H28" s="54"/>
+      <c r="H28" s="43"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="40">
+      <c r="D29" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="28">
         <v>8</v>
       </c>
-      <c r="F29" s="40">
+      <c r="F29" s="28">
         <v>5</v>
       </c>
-      <c r="G29" s="57">
+      <c r="G29" s="37">
         <v>44345</v>
       </c>
-      <c r="H29" s="54"/>
+      <c r="H29" s="43"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="40">
+      <c r="D30" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="28">
         <v>8</v>
       </c>
-      <c r="F30" s="40">
+      <c r="F30" s="28">
         <v>7</v>
       </c>
-      <c r="G30" s="57">
+      <c r="G30" s="37">
         <v>44345</v>
       </c>
-      <c r="H30" s="56"/>
+      <c r="H30" s="44"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="40">
+      <c r="D31" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="28">
         <v>21</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="28">
         <v>8</v>
       </c>
-      <c r="G31" s="57">
+      <c r="G31" s="37">
         <v>44346</v>
       </c>
-      <c r="H31" s="56"/>
+      <c r="H31" s="44"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="40">
+      <c r="D32" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="28">
         <v>8</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="28">
         <v>9</v>
       </c>
-      <c r="G32" s="57">
+      <c r="G32" s="37">
         <v>44346</v>
       </c>
-      <c r="H32" s="55"/>
+      <c r="H32" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>